<commit_message>
FIX quickdrive not working
</commit_message>
<xml_diff>
--- a/RailWorks/Source/RailionLudmilla-Consists/Quickdrive/overzicht.xlsx
+++ b/RailWorks/Source/RailionLudmilla-Consists/Quickdrive/overzicht.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\RailWorks\Source\RailionLudmilla-Consists\Quickdrive\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Games\Steam\steamapps\common\RailWorks\Source\RailionLudmilla-Consists\Quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4903022-A1C5-4259-9E61-EF0C0DB55F08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C9DD9BB-0F11-4DC2-8608-6A0CAC35243C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Voorstel Universeel Testje" sheetId="7" r:id="rId1"/>
@@ -65,6 +65,30 @@
           </rPr>
           <t xml:space="preserve">
 Geel: indien nodig toewijzen aan Custom X</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{A92C6D3D-A459-4D2D-8346-5976CFFCDDF5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Groen: ingevoerd en compleet</t>
         </r>
       </text>
     </comment>
@@ -905,7 +929,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -953,8 +977,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -973,6 +1010,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -986,7 +1029,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1007,7 +1050,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1293,10 +1339,10 @@
   <dimension ref="A1:AY46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="J3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="N28" sqref="N28:AX36"/>
+      <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1460,7 +1506,7 @@
     </row>
     <row r="2" spans="1:51" x14ac:dyDescent="0.45">
       <c r="A2" s="5"/>
-      <c r="B2" s="1"/>
+      <c r="B2" s="13"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -1569,7 +1615,7 @@
       <c r="A3" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="12" t="s">
         <v>85</v>
       </c>
       <c r="C3" t="s">

</xml_diff>

<commit_message>
QD consists DDZ, IRM
</commit_message>
<xml_diff>
--- a/RailWorks/Source/RailionLudmilla-Consists/Quickdrive/overzicht.xlsx
+++ b/RailWorks/Source/RailionLudmilla-Consists/Quickdrive/overzicht.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Games\Steam\steamapps\common\RailWorks\Source\RailionLudmilla-Consists\Quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C9DD9BB-0F11-4DC2-8608-6A0CAC35243C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64D61158-573F-4E7F-BFB0-034312C66869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1470" yWindow="1470" windowWidth="15248" windowHeight="11648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Voorstel Universeel Testje" sheetId="7" r:id="rId1"/>
@@ -1029,7 +1029,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1056,6 +1056,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -1342,7 +1343,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
+      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1691,10 +1692,10 @@
       <c r="AY3" s="4"/>
     </row>
     <row r="4" spans="1:51" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
+      <c r="A4" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="14" t="s">
         <v>68</v>
       </c>
       <c r="C4" t="s">

</xml_diff>